<commit_message>
Cambios en ubicación de recursos
Cambios en ubicación de recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion12/ESCALETA FINAL CN_11_12_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion12/ESCALETA FINAL CN_11_12_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -11,9 +16,9 @@
     <sheet name="DATOS" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$U$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$U$40</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="216">
   <si>
     <t>Asignatura</t>
   </si>
@@ -397,9 +402,6 @@
     <t>Competencias</t>
   </si>
   <si>
-    <t xml:space="preserve">Los alcoholes </t>
-  </si>
-  <si>
     <t>RF</t>
   </si>
   <si>
@@ -418,9 +420,6 @@
     <t>Recurso F13B-01</t>
   </si>
   <si>
-    <t>Los aldehídos y cetonas</t>
-  </si>
-  <si>
     <t xml:space="preserve">Interactivo que muestra las generalidades de los aldehídos y las cetonas </t>
   </si>
   <si>
@@ -430,9 +429,6 @@
     <t xml:space="preserve">Interactivo que permite obtener experimentalmente un alcohol y determinar los tipos de alcoholes </t>
   </si>
   <si>
-    <t xml:space="preserve">Interactivo que permite mostrar las generalidades de los ácidos carboxílicos </t>
-  </si>
-  <si>
     <t>Recurso F6-03</t>
   </si>
   <si>
@@ -562,12 +558,6 @@
     <t>Recurso M1D-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Escribe los nombres  de los aldehídos y cetonas </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividad que permite practicar la nomenclatura de los aldehídos y las cetonas </t>
-  </si>
-  <si>
     <t>Recurso M6A-02</t>
   </si>
   <si>
@@ -616,15 +606,9 @@
     <t>Recurso M5A-01</t>
   </si>
   <si>
-    <t>Los éteres</t>
-  </si>
-  <si>
     <t>Secuencia de imágenes que permite explicar las generalidades de los éteres</t>
   </si>
   <si>
-    <t>Diaporama F1-02</t>
-  </si>
-  <si>
     <t xml:space="preserve">Actividad que permite ejercitar la nomenclatura de los alcoholes </t>
   </si>
   <si>
@@ -658,17 +642,56 @@
     <t xml:space="preserve">Actividad que propone realizar una práctica de laboratorio para extraer aceite de origen vegetal </t>
   </si>
   <si>
-    <t>Diaporama F1-03</t>
-  </si>
-  <si>
     <t>Diaporama F1-04</t>
+  </si>
+  <si>
+    <t>Recurso FQ_10_13_08-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los alcoholes aromáticos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactivo que permite explicar las características y propiedades de los fenoles </t>
+  </si>
+  <si>
+    <t>Recurso F7B-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secuencia </t>
+  </si>
+  <si>
+    <t>Los aldehídos y las cetonas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Escribe los nombres de los aldehídos  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad que permite practicar la nomenclatura de los aldehídos </t>
+  </si>
+  <si>
+    <t>Recurso FQ_10_13_08-02</t>
+  </si>
+  <si>
+    <t>FQ_10_13</t>
+  </si>
+  <si>
+    <t>La función alcohol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los ácidos orgánicos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactivo que permite mostrar las generalidades de los ácidos orgánicos o carboxílicos </t>
+  </si>
+  <si>
+    <t>La función éter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -696,8 +719,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -743,6 +773,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1011,7 +1065,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1088,6 +1142,91 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1384,7 +1523,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1392,10 +1531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U94"/>
+  <dimension ref="A1:U98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,7 +1544,7 @@
     <col min="3" max="3" width="32.85546875" customWidth="1"/>
     <col min="4" max="4" width="45.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.140625" customWidth="1"/>
     <col min="7" max="7" width="63.42578125" customWidth="1"/>
     <col min="8" max="9" width="11.42578125" style="5"/>
     <col min="10" max="10" width="92.28515625" customWidth="1"/>
@@ -1423,94 +1562,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="103" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="54" t="s">
+      <c r="M1" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="48" t="s">
+      <c r="N1" s="106"/>
+      <c r="O1" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="48" t="s">
+      <c r="P1" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="Q1" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="48" t="s">
+      <c r="R1" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="48" t="s">
+      <c r="S1" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="48" t="s">
+      <c r="T1" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="48" t="s">
+      <c r="U1" s="99" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="10" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="51"/>
+      <c r="A2" s="100"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="102"/>
       <c r="M2" s="47" t="s">
         <v>87</v>
       </c>
       <c r="N2" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
+      <c r="O2" s="100"/>
+      <c r="P2" s="100"/>
+      <c r="Q2" s="100"/>
+      <c r="R2" s="100"/>
+      <c r="S2" s="100"/>
+      <c r="T2" s="100"/>
+      <c r="U2" s="100"/>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
@@ -1525,12 +1664,10 @@
       <c r="D3" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E3" s="42" t="s">
-        <v>93</v>
-      </c>
+      <c r="E3" s="42"/>
       <c r="F3" s="24"/>
       <c r="G3" s="29" t="s">
-        <v>121</v>
+        <v>212</v>
       </c>
       <c r="H3" s="30">
         <v>1</v>
@@ -1539,7 +1676,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="31" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="K3" s="35" t="s">
         <v>69</v>
@@ -1559,16 +1696,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="S3" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="T3" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="T3" s="11" t="s">
+      <c r="U3" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1584,109 +1721,83 @@
       <c r="D4" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="24"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="2"/>
+    </row>
+    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="32" t="s">
-        <v>168</v>
-      </c>
-      <c r="H4" s="33">
+      <c r="F5" s="53"/>
+      <c r="G5" s="54" t="s">
+        <v>165</v>
+      </c>
+      <c r="H5" s="55">
         <v>2</v>
       </c>
-      <c r="I4" s="33" t="s">
+      <c r="I5" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="34" t="s">
-        <v>197</v>
-      </c>
-      <c r="K4" s="37" t="s">
+      <c r="J5" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="K5" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="38" t="s">
+      <c r="L5" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4" s="41"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="39" t="s">
+      <c r="M5" s="58"/>
+      <c r="N5" s="58" t="s">
+        <v>211</v>
+      </c>
+      <c r="O5" s="59"/>
+      <c r="P5" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="Q5" s="61">
         <v>6</v>
       </c>
-      <c r="R4" s="11" t="s">
+      <c r="R5" s="61" t="s">
+        <v>134</v>
+      </c>
+      <c r="S5" s="62" t="s">
+        <v>135</v>
+      </c>
+      <c r="T5" s="63" t="s">
+        <v>202</v>
+      </c>
+      <c r="U5" s="61" t="s">
         <v>137</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="T4" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="H5" s="33">
-        <v>3</v>
-      </c>
-      <c r="I5" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="34" t="s">
-        <v>173</v>
-      </c>
-      <c r="K5" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="L5" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="O5" s="40"/>
-      <c r="P5" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>6</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="T5" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -1703,31 +1814,31 @@
         <v>92</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F6" s="26"/>
-      <c r="G6" s="46" t="s">
-        <v>126</v>
+      <c r="G6" s="32" t="s">
+        <v>169</v>
       </c>
       <c r="H6" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I6" s="33" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J6" s="34" t="s">
-        <v>131</v>
+        <v>170</v>
       </c>
       <c r="K6" s="37" t="s">
         <v>69</v>
       </c>
       <c r="L6" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="M6" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="N6" s="41"/>
+        <v>32</v>
+      </c>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41" t="s">
+        <v>76</v>
+      </c>
       <c r="O6" s="40"/>
       <c r="P6" s="39" t="s">
         <v>19</v>
@@ -1736,16 +1847,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="S6" s="11" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>127</v>
+        <v>171</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -1766,45 +1877,45 @@
       </c>
       <c r="F7" s="26"/>
       <c r="G7" s="46" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
       <c r="H7" s="33">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I7" s="33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J7" s="34" t="s">
-        <v>180</v>
+        <v>129</v>
       </c>
       <c r="K7" s="37" t="s">
         <v>69</v>
       </c>
       <c r="L7" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="M7" s="41"/>
-      <c r="N7" s="41" t="s">
-        <v>24</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="M7" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" s="41"/>
       <c r="O7" s="40"/>
       <c r="P7" s="39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q7" s="1">
         <v>6</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>181</v>
+        <v>126</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -1820,21 +1931,21 @@
       <c r="D8" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E8" s="43" t="s">
-        <v>97</v>
+      <c r="E8" s="25" t="s">
+        <v>96</v>
       </c>
       <c r="F8" s="26"/>
-      <c r="G8" s="32" t="s">
-        <v>144</v>
+      <c r="G8" s="46" t="s">
+        <v>174</v>
       </c>
       <c r="H8" s="33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I8" s="33" t="s">
         <v>20</v>
       </c>
       <c r="J8" s="34" t="s">
-        <v>145</v>
+        <v>175</v>
       </c>
       <c r="K8" s="37" t="s">
         <v>69</v>
@@ -1844,26 +1955,26 @@
       </c>
       <c r="M8" s="41"/>
       <c r="N8" s="41" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="O8" s="40"/>
       <c r="P8" s="39" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q8" s="1">
         <v>6</v>
       </c>
       <c r="R8" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="T8" s="11" t="s">
-        <v>146</v>
+        <v>176</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -1876,24 +1987,24 @@
       <c r="C9" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D9" s="22" t="s">
-        <v>98</v>
+      <c r="D9" s="18" t="s">
+        <v>92</v>
       </c>
       <c r="E9" s="43" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F9" s="26"/>
       <c r="G9" s="32" t="s">
-        <v>198</v>
+        <v>141</v>
       </c>
       <c r="H9" s="33">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I9" s="33" t="s">
         <v>20</v>
       </c>
       <c r="J9" s="34" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="K9" s="37" t="s">
         <v>69</v>
@@ -1903,7 +2014,7 @@
       </c>
       <c r="M9" s="41"/>
       <c r="N9" s="41" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="O9" s="40"/>
       <c r="P9" s="39" t="s">
@@ -1913,50 +2024,74 @@
         <v>6</v>
       </c>
       <c r="R9" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="S9" s="11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="T9" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="67" t="s">
         <v>98</v>
       </c>
-      <c r="E10" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="2"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="67" t="s">
+        <v>203</v>
+      </c>
+      <c r="H10" s="70">
+        <v>7</v>
+      </c>
+      <c r="I10" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="71" t="s">
+        <v>204</v>
+      </c>
+      <c r="K10" s="72" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" s="73" t="s">
+        <v>31</v>
+      </c>
+      <c r="M10" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="N10" s="74"/>
+      <c r="O10" s="75"/>
+      <c r="P10" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="77">
+        <v>6</v>
+      </c>
+      <c r="R10" s="77" t="s">
+        <v>121</v>
+      </c>
+      <c r="S10" s="77" t="s">
+        <v>122</v>
+      </c>
+      <c r="T10" s="78" t="s">
+        <v>205</v>
+      </c>
+      <c r="U10" s="77" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
@@ -1971,25 +2106,51 @@
       <c r="D11" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="E11" s="25" t="s">
-        <v>101</v>
+      <c r="E11" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="F11" s="26"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="38"/>
+      <c r="G11" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="H11" s="33">
+        <v>8</v>
+      </c>
+      <c r="I11" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="K11" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" s="38" t="s">
+        <v>32</v>
+      </c>
       <c r="M11" s="41"/>
-      <c r="N11" s="41"/>
+      <c r="N11" s="41" t="s">
+        <v>47</v>
+      </c>
       <c r="O11" s="40"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="2"/>
+      <c r="P11" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>6</v>
+      </c>
+      <c r="R11" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="S11" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="T11" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
@@ -2004,53 +2165,27 @@
       <c r="D12" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="E12" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="H12" s="33">
-        <v>8</v>
-      </c>
-      <c r="I12" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="34" t="s">
-        <v>148</v>
-      </c>
-      <c r="K12" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="L12" s="38" t="s">
-        <v>32</v>
-      </c>
+      <c r="E12" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="F12" s="24"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="38"/>
       <c r="M12" s="41"/>
-      <c r="N12" s="41" t="s">
-        <v>62</v>
-      </c>
+      <c r="N12" s="41"/>
       <c r="O12" s="40"/>
-      <c r="P12" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q12" s="1">
-        <v>6</v>
-      </c>
-      <c r="R12" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="S12" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="T12" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P12" s="39"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="2"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>67</v>
       </c>
@@ -2060,56 +2195,30 @@
       <c r="C13" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="45" t="s">
-        <v>103</v>
+      <c r="D13" s="22" t="s">
+        <v>98</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F13" s="26"/>
-      <c r="G13" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="H13" s="33">
-        <v>9</v>
-      </c>
-      <c r="I13" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="K13" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="L13" s="38" t="s">
-        <v>32</v>
-      </c>
+      <c r="G13" s="32"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="38"/>
       <c r="M13" s="41"/>
-      <c r="N13" s="41" t="s">
-        <v>75</v>
-      </c>
+      <c r="N13" s="41"/>
       <c r="O13" s="40"/>
-      <c r="P13" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>6</v>
-      </c>
-      <c r="R13" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="S13" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="T13" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P13" s="39"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="2"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>67</v>
       </c>
@@ -2119,87 +2228,113 @@
       <c r="C14" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="45" t="s">
+      <c r="D14" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" s="26"/>
+      <c r="G14" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="H14" s="33">
+        <v>9</v>
+      </c>
+      <c r="I14" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="K14" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="L14" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="O14" s="40"/>
+      <c r="P14" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>6</v>
+      </c>
+      <c r="R14" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="S14" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="T14" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="79" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="80" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="81" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="94" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="F14" s="26"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="40"/>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
-      <c r="U14" s="2"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="32" t="s">
-        <v>194</v>
-      </c>
-      <c r="H15" s="33">
+      <c r="E15" s="83"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="82" t="s">
+        <v>215</v>
+      </c>
+      <c r="H15" s="85">
         <v>10</v>
       </c>
-      <c r="I15" s="33" t="s">
+      <c r="I15" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="34" t="s">
-        <v>195</v>
-      </c>
-      <c r="K15" s="37" t="s">
+      <c r="J15" s="86" t="s">
+        <v>189</v>
+      </c>
+      <c r="K15" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="L15" s="38"/>
-      <c r="M15" s="41" t="s">
+      <c r="L15" s="87" t="s">
+        <v>206</v>
+      </c>
+      <c r="M15" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="N15" s="41"/>
-      <c r="O15" s="40" t="s">
+      <c r="N15" s="88"/>
+      <c r="O15" s="89" t="s">
+        <v>133</v>
+      </c>
+      <c r="P15" s="90"/>
+      <c r="Q15" s="91">
+        <v>6</v>
+      </c>
+      <c r="R15" s="92" t="s">
+        <v>134</v>
+      </c>
+      <c r="S15" s="92" t="s">
+        <v>135</v>
+      </c>
+      <c r="T15" s="92" t="s">
         <v>136</v>
       </c>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="1">
-        <v>6</v>
-      </c>
-      <c r="R15" s="11" t="s">
+      <c r="U15" s="93" t="s">
         <v>137</v>
       </c>
-      <c r="S15" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="T15" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="U15" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>67</v>
       </c>
@@ -2213,11 +2348,11 @@
         <v>103</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F16" s="26"/>
       <c r="G16" s="32" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="H16" s="33">
         <v>11</v>
@@ -2226,7 +2361,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="34" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="K16" s="37" t="s">
         <v>69</v>
@@ -2236,7 +2371,7 @@
       </c>
       <c r="M16" s="41"/>
       <c r="N16" s="41" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="O16" s="40"/>
       <c r="P16" s="39" t="s">
@@ -2246,19 +2381,19 @@
         <v>6</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="S16" s="11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="T16" s="11" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>67</v>
       </c>
@@ -2269,14 +2404,12 @@
         <v>91</v>
       </c>
       <c r="D17" s="45" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>109</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="F17" s="26"/>
       <c r="G17" s="32"/>
       <c r="H17" s="33"/>
       <c r="I17" s="33"/>
@@ -2304,14 +2437,12 @@
         <v>91</v>
       </c>
       <c r="D18" s="45" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>110</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="F18" s="26"/>
       <c r="G18" s="32"/>
       <c r="H18" s="33"/>
       <c r="I18" s="33"/>
@@ -2339,125 +2470,173 @@
         <v>91</v>
       </c>
       <c r="D19" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="26"/>
+      <c r="G19" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="H19" s="33">
+        <v>12</v>
+      </c>
+      <c r="I19" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="K19" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="L19" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="O19" s="40"/>
+      <c r="P19" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>6</v>
+      </c>
+      <c r="R19" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="S19" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="T19" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="U19" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="79" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="80" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="81" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="94" t="s">
         <v>107</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="E20" s="83" t="s">
         <v>108</v>
       </c>
-      <c r="F19" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="G19" s="32"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="41"/>
-      <c r="N19" s="41"/>
-      <c r="O19" s="40"/>
-      <c r="P19" s="39"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
-      <c r="U19" s="2"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="F20" s="84"/>
+      <c r="G20" s="82" t="s">
+        <v>207</v>
+      </c>
+      <c r="H20" s="85">
+        <v>13</v>
+      </c>
+      <c r="I20" s="85" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="86" t="s">
+        <v>127</v>
+      </c>
+      <c r="K20" s="83" t="s">
+        <v>69</v>
+      </c>
+      <c r="L20" s="87" t="s">
+        <v>31</v>
+      </c>
+      <c r="M20" s="88" t="s">
+        <v>36</v>
+      </c>
+      <c r="N20" s="88"/>
+      <c r="O20" s="89"/>
+      <c r="P20" s="90" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q20" s="91">
+        <v>6</v>
+      </c>
+      <c r="R20" s="92" t="s">
+        <v>121</v>
+      </c>
+      <c r="S20" s="92" t="s">
+        <v>122</v>
+      </c>
+      <c r="T20" s="92" t="s">
+        <v>128</v>
+      </c>
+      <c r="U20" s="93" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B21" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C21" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="45" t="s">
+      <c r="D21" s="94" t="s">
         <v>107</v>
       </c>
-      <c r="E20" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="F20" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="G20" s="32" t="s">
-        <v>199</v>
-      </c>
-      <c r="H20" s="33">
-        <v>12</v>
-      </c>
-      <c r="I20" s="33" t="s">
+      <c r="E21" s="83" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" s="84" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21" s="82" t="s">
+        <v>208</v>
+      </c>
+      <c r="H21" s="85">
+        <v>14</v>
+      </c>
+      <c r="I21" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="K20" s="37" t="s">
+      <c r="J21" s="86" t="s">
+        <v>209</v>
+      </c>
+      <c r="K21" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="L20" s="38" t="s">
+      <c r="L21" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="O20" s="40"/>
-      <c r="P20" s="39" t="s">
+      <c r="M21" s="88"/>
+      <c r="N21" s="88" t="s">
+        <v>47</v>
+      </c>
+      <c r="O21" s="89"/>
+      <c r="P21" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="1">
+      <c r="Q21" s="91">
         <v>6</v>
       </c>
-      <c r="R20" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="S20" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="T20" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="U20" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D21" s="45" t="s">
-        <v>107</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="F21" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="G21" s="32"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="41"/>
-      <c r="N21" s="41"/>
-      <c r="O21" s="40"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="11"/>
-      <c r="T21" s="11"/>
-      <c r="U21" s="2"/>
+      <c r="R21" s="92" t="s">
+        <v>134</v>
+      </c>
+      <c r="S21" s="92" t="s">
+        <v>138</v>
+      </c>
+      <c r="T21" s="92" t="s">
+        <v>173</v>
+      </c>
+      <c r="U21" s="93" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
@@ -2473,52 +2652,26 @@
         <v>107</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="G22" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="H22" s="33">
-        <v>13</v>
-      </c>
-      <c r="I22" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="J22" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="K22" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="L22" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="M22" s="41" t="s">
-        <v>36</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="G22" s="32"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="41"/>
       <c r="N22" s="41"/>
       <c r="O22" s="40"/>
-      <c r="P22" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q22" s="1">
-        <v>6</v>
-      </c>
-      <c r="R22" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="S22" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="T22" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="U22" s="2" t="s">
-        <v>125</v>
-      </c>
+      <c r="P22" s="39"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="2"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
@@ -2534,54 +2687,28 @@
         <v>107</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F23" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="G23" s="32" t="s">
-        <v>176</v>
-      </c>
-      <c r="H23" s="33">
-        <v>14</v>
-      </c>
-      <c r="I23" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J23" s="34" t="s">
-        <v>177</v>
-      </c>
-      <c r="K23" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="L23" s="38" t="s">
-        <v>32</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="G23" s="32"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="38"/>
       <c r="M23" s="41"/>
-      <c r="N23" s="41" t="s">
-        <v>47</v>
-      </c>
+      <c r="N23" s="41"/>
       <c r="O23" s="40"/>
-      <c r="P23" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q23" s="1">
-        <v>6</v>
-      </c>
-      <c r="R23" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="S23" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="T23" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="U23" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="P23" s="39"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="2"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>67</v>
       </c>
@@ -2595,20 +2722,22 @@
         <v>107</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="F24" s="26"/>
-      <c r="G24" s="46" t="s">
-        <v>154</v>
+        <v>112</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G24" s="32" t="s">
+        <v>192</v>
       </c>
       <c r="H24" s="33">
         <v>15</v>
       </c>
       <c r="I24" s="33" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J24" s="34" t="s">
-        <v>155</v>
+        <v>193</v>
       </c>
       <c r="K24" s="37" t="s">
         <v>69</v>
@@ -2618,7 +2747,7 @@
       </c>
       <c r="M24" s="41"/>
       <c r="N24" s="41" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="O24" s="40"/>
       <c r="P24" s="39" t="s">
@@ -2628,16 +2757,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="S24" s="11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="T24" s="11" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -2650,54 +2779,30 @@
       <c r="C25" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D25" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="E25" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="F25" s="26"/>
-      <c r="G25" s="32" t="s">
-        <v>182</v>
-      </c>
-      <c r="H25" s="33">
-        <v>16</v>
-      </c>
-      <c r="I25" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" s="34" t="s">
-        <v>201</v>
-      </c>
-      <c r="K25" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="L25" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="M25" s="41" t="s">
-        <v>34</v>
-      </c>
+      <c r="D25" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="G25" s="32"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="41"/>
       <c r="N25" s="41"/>
       <c r="O25" s="40"/>
-      <c r="P25" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q25" s="1">
-        <v>6</v>
-      </c>
-      <c r="R25" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="S25" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="T25" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="U25" s="2" t="s">
-        <v>140</v>
-      </c>
+      <c r="P25" s="39"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="2"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
@@ -2709,56 +2814,32 @@
       <c r="C26" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D26" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="E26" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="F26" s="26"/>
-      <c r="G26" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="H26" s="33">
-        <v>17</v>
-      </c>
-      <c r="I26" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="J26" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="K26" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="L26" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="M26" s="41" t="s">
-        <v>36</v>
-      </c>
+      <c r="D26" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="G26" s="32"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="41"/>
       <c r="N26" s="41"/>
       <c r="O26" s="40"/>
-      <c r="P26" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q26" s="1">
-        <v>6</v>
-      </c>
-      <c r="R26" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="S26" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="T26" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="U26" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P26" s="39"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="2"/>
+    </row>
+    <row r="27" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>67</v>
       </c>
@@ -2768,36 +2849,36 @@
       <c r="C27" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D27" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="E27" s="43" t="s">
-        <v>119</v>
+      <c r="D27" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>102</v>
       </c>
       <c r="F27" s="26"/>
-      <c r="G27" s="32" t="s">
-        <v>134</v>
+      <c r="G27" s="46" t="s">
+        <v>151</v>
       </c>
       <c r="H27" s="33">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I27" s="33" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J27" s="34" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="K27" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="L27" s="38"/>
-      <c r="M27" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="N27" s="41"/>
-      <c r="O27" s="40" t="s">
-        <v>136</v>
-      </c>
+      <c r="L27" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="O27" s="40"/>
       <c r="P27" s="39" t="s">
         <v>19</v>
       </c>
@@ -2805,13 +2886,13 @@
         <v>6</v>
       </c>
       <c r="R27" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="S27" s="11" t="s">
         <v>138</v>
       </c>
       <c r="T27" s="11" t="s">
-        <v>209</v>
+        <v>153</v>
       </c>
       <c r="U27" s="2" t="s">
         <v>140</v>
@@ -2830,32 +2911,30 @@
       <c r="D28" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="E28" s="25" t="s">
-        <v>102</v>
-      </c>
+      <c r="E28" s="43"/>
       <c r="F28" s="26"/>
-      <c r="G28" s="46" t="s">
-        <v>151</v>
+      <c r="G28" s="32" t="s">
+        <v>213</v>
       </c>
       <c r="H28" s="33">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I28" s="33" t="s">
         <v>19</v>
       </c>
       <c r="J28" s="34" t="s">
-        <v>157</v>
+        <v>214</v>
       </c>
       <c r="K28" s="37" t="s">
         <v>69</v>
       </c>
       <c r="L28" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="M28" s="41"/>
-      <c r="N28" s="41" t="s">
-        <v>62</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="M28" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="N28" s="41"/>
       <c r="O28" s="40"/>
       <c r="P28" s="39" t="s">
         <v>19</v>
@@ -2864,76 +2943,78 @@
         <v>6</v>
       </c>
       <c r="R28" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="S28" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="T28" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="U28" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="E29" s="97" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="53"/>
+      <c r="G29" s="54" t="s">
+        <v>177</v>
+      </c>
+      <c r="H29" s="55">
+        <v>18</v>
+      </c>
+      <c r="I29" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" s="56" t="s">
+        <v>194</v>
+      </c>
+      <c r="K29" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="L29" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="M29" s="58"/>
+      <c r="N29" s="58" t="s">
+        <v>211</v>
+      </c>
+      <c r="O29" s="59"/>
+      <c r="P29" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q29" s="61">
+        <v>6</v>
+      </c>
+      <c r="R29" s="61" t="s">
+        <v>134</v>
+      </c>
+      <c r="S29" s="62" t="s">
+        <v>135</v>
+      </c>
+      <c r="T29" s="63" t="s">
+        <v>210</v>
+      </c>
+      <c r="U29" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="S28" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="T28" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="U28" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="E29" s="25"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="32" t="s">
-        <v>184</v>
-      </c>
-      <c r="H29" s="33">
-        <v>20</v>
-      </c>
-      <c r="I29" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J29" s="34" t="s">
-        <v>185</v>
-      </c>
-      <c r="K29" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="L29" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="M29" s="41"/>
-      <c r="N29" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="O29" s="40"/>
-      <c r="P29" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q29" s="1">
-        <v>6</v>
-      </c>
-      <c r="R29" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="S29" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="T29" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="U29" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>67</v>
       </c>
@@ -2944,53 +3025,29 @@
         <v>91</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="E30" s="25"/>
+        <v>116</v>
+      </c>
+      <c r="E30" s="43" t="s">
+        <v>118</v>
+      </c>
       <c r="F30" s="26"/>
-      <c r="G30" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="H30" s="33">
-        <v>21</v>
-      </c>
-      <c r="I30" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J30" s="34" t="s">
-        <v>160</v>
-      </c>
-      <c r="K30" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="L30" s="38" t="s">
-        <v>32</v>
-      </c>
+      <c r="G30" s="32"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="38"/>
       <c r="M30" s="41"/>
-      <c r="N30" s="41" t="s">
-        <v>64</v>
-      </c>
+      <c r="N30" s="41"/>
       <c r="O30" s="40"/>
-      <c r="P30" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q30" s="1">
-        <v>6</v>
-      </c>
-      <c r="R30" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="S30" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="T30" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="U30" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P30" s="39"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="2"/>
+    </row>
+    <row r="31" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>67</v>
       </c>
@@ -3001,33 +3058,35 @@
         <v>91</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="E31" s="25"/>
+        <v>116</v>
+      </c>
+      <c r="E31" s="43" t="s">
+        <v>119</v>
+      </c>
       <c r="F31" s="26"/>
       <c r="G31" s="32" t="s">
-        <v>202</v>
+        <v>131</v>
       </c>
       <c r="H31" s="33">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I31" s="33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J31" s="34" t="s">
-        <v>207</v>
+        <v>132</v>
       </c>
       <c r="K31" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="L31" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="M31" s="41"/>
-      <c r="N31" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="O31" s="40"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="N31" s="41"/>
+      <c r="O31" s="40" t="s">
+        <v>133</v>
+      </c>
       <c r="P31" s="39" t="s">
         <v>19</v>
       </c>
@@ -3035,130 +3094,134 @@
         <v>6</v>
       </c>
       <c r="R31" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="S31" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="T31" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="U31" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="S31" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="T31" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="U31" s="2" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="D32" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="E32" s="25"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="32" t="s">
+      <c r="D32" s="82" t="s">
+        <v>116</v>
+      </c>
+      <c r="E32" s="98" t="s">
+        <v>119</v>
+      </c>
+      <c r="F32" s="84"/>
+      <c r="G32" s="82" t="s">
+        <v>182</v>
+      </c>
+      <c r="H32" s="85">
+        <v>20</v>
+      </c>
+      <c r="I32" s="85" t="s">
+        <v>20</v>
+      </c>
+      <c r="J32" s="86" t="s">
+        <v>183</v>
+      </c>
+      <c r="K32" s="83" t="s">
+        <v>69</v>
+      </c>
+      <c r="L32" s="87" t="s">
+        <v>32</v>
+      </c>
+      <c r="M32" s="88"/>
+      <c r="N32" s="88" t="s">
+        <v>53</v>
+      </c>
+      <c r="O32" s="89"/>
+      <c r="P32" s="90" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q32" s="91">
+        <v>6</v>
+      </c>
+      <c r="R32" s="92" t="s">
+        <v>134</v>
+      </c>
+      <c r="S32" s="92" t="s">
+        <v>138</v>
+      </c>
+      <c r="T32" s="92" t="s">
+        <v>184</v>
+      </c>
+      <c r="U32" s="93" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="79" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="80" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="81" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="82" t="s">
+        <v>116</v>
+      </c>
+      <c r="E33" s="98" t="s">
+        <v>119</v>
+      </c>
+      <c r="F33" s="84"/>
+      <c r="G33" s="82" t="s">
+        <v>185</v>
+      </c>
+      <c r="H33" s="85">
+        <v>21</v>
+      </c>
+      <c r="I33" s="85" t="s">
+        <v>20</v>
+      </c>
+      <c r="J33" s="86" t="s">
+        <v>186</v>
+      </c>
+      <c r="K33" s="83" t="s">
+        <v>69</v>
+      </c>
+      <c r="L33" s="87" t="s">
+        <v>32</v>
+      </c>
+      <c r="M33" s="88"/>
+      <c r="N33" s="88" t="s">
+        <v>47</v>
+      </c>
+      <c r="O33" s="89"/>
+      <c r="P33" s="90" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q33" s="91">
+        <v>6</v>
+      </c>
+      <c r="R33" s="92" t="s">
+        <v>134</v>
+      </c>
+      <c r="S33" s="92" t="s">
+        <v>138</v>
+      </c>
+      <c r="T33" s="92" t="s">
         <v>187</v>
       </c>
-      <c r="H32" s="33">
-        <v>23</v>
-      </c>
-      <c r="I32" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J32" s="34" t="s">
-        <v>188</v>
-      </c>
-      <c r="K32" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="L32" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="M32" s="41"/>
-      <c r="N32" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="O32" s="40"/>
-      <c r="P32" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q32" s="1">
-        <v>6</v>
-      </c>
-      <c r="R32" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="S32" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="T32" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="U32" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="E33" s="25"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="H33" s="33">
-        <v>24</v>
-      </c>
-      <c r="I33" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J33" s="34" t="s">
-        <v>191</v>
-      </c>
-      <c r="K33" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="L33" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="M33" s="41"/>
-      <c r="N33" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="O33" s="40"/>
-      <c r="P33" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q33" s="1">
-        <v>6</v>
-      </c>
-      <c r="R33" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="S33" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="T33" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="U33" s="2" t="s">
-        <v>143</v>
+      <c r="U33" s="93" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -3172,41 +3235,55 @@
         <v>91</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="E34" s="25"/>
+        <v>116</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>102</v>
+      </c>
       <c r="F34" s="26"/>
-      <c r="G34" s="32" t="s">
-        <v>164</v>
+      <c r="G34" s="46" t="s">
+        <v>148</v>
       </c>
       <c r="H34" s="33">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I34" s="33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J34" s="34" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="K34" s="37" t="s">
         <v>69</v>
       </c>
       <c r="L34" s="38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M34" s="41"/>
-      <c r="N34" s="41"/>
+      <c r="N34" s="41" t="s">
+        <v>62</v>
+      </c>
       <c r="O34" s="40"/>
       <c r="P34" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="11"/>
-      <c r="S34" s="11"/>
-      <c r="T34" s="11"/>
-      <c r="U34" s="2"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q34" s="1">
+        <v>6</v>
+      </c>
+      <c r="R34" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="S34" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="T34" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="U34" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
         <v>67</v>
       </c>
@@ -3217,21 +3294,21 @@
         <v>91</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="E35" s="25"/>
       <c r="F35" s="26"/>
       <c r="G35" s="32" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="H35" s="33">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I35" s="33" t="s">
         <v>20</v>
       </c>
       <c r="J35" s="34" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="K35" s="37" t="s">
         <v>69</v>
@@ -3241,7 +3318,7 @@
       </c>
       <c r="M35" s="41"/>
       <c r="N35" s="41" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="O35" s="40"/>
       <c r="P35" s="39" t="s">
@@ -3251,19 +3328,19 @@
         <v>6</v>
       </c>
       <c r="R35" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="S35" s="11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="T35" s="11" t="s">
-        <v>193</v>
+        <v>158</v>
       </c>
       <c r="U35" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>67</v>
       </c>
@@ -3273,20 +3350,22 @@
       <c r="C36" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D36" s="22"/>
+      <c r="D36" s="22" t="s">
+        <v>120</v>
+      </c>
       <c r="E36" s="25"/>
       <c r="F36" s="26"/>
       <c r="G36" s="32" t="s">
-        <v>205</v>
+        <v>156</v>
       </c>
       <c r="H36" s="33">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I36" s="33" t="s">
         <v>20</v>
       </c>
       <c r="J36" s="34" t="s">
-        <v>206</v>
+        <v>157</v>
       </c>
       <c r="K36" s="37" t="s">
         <v>69</v>
@@ -3296,68 +3375,124 @@
       </c>
       <c r="M36" s="41"/>
       <c r="N36" s="41" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O36" s="40"/>
       <c r="P36" s="39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q36" s="1">
         <v>6</v>
       </c>
       <c r="R36" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="S36" s="11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="T36" s="11" t="s">
-        <v>204</v>
+        <v>159</v>
       </c>
       <c r="U36" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="22"/>
+      <c r="A37" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>120</v>
+      </c>
       <c r="E37" s="25"/>
       <c r="F37" s="26"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="33"/>
-      <c r="I37" s="33"/>
-      <c r="J37" s="34"/>
-      <c r="K37" s="37"/>
-      <c r="L37" s="38"/>
+      <c r="G37" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="H37" s="33">
+        <v>25</v>
+      </c>
+      <c r="I37" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J37" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="K37" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="L37" s="38" t="s">
+        <v>32</v>
+      </c>
       <c r="M37" s="41"/>
-      <c r="N37" s="41"/>
+      <c r="N37" s="41" t="s">
+        <v>64</v>
+      </c>
       <c r="O37" s="40"/>
-      <c r="P37" s="39"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="11"/>
-      <c r="S37" s="11"/>
-      <c r="T37" s="11"/>
-      <c r="U37" s="2"/>
+      <c r="P37" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>6</v>
+      </c>
+      <c r="R37" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="S37" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="T37" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="U37" s="2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="22"/>
+      <c r="A38" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>160</v>
+      </c>
       <c r="E38" s="25"/>
       <c r="F38" s="26"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="34"/>
-      <c r="K38" s="37"/>
-      <c r="L38" s="38"/>
+      <c r="G38" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="H38" s="33">
+        <v>26</v>
+      </c>
+      <c r="I38" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="K38" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="L38" s="38" t="s">
+        <v>33</v>
+      </c>
       <c r="M38" s="41"/>
       <c r="N38" s="41"/>
       <c r="O38" s="40"/>
-      <c r="P38" s="39"/>
+      <c r="P38" s="39" t="s">
+        <v>19</v>
+      </c>
       <c r="Q38" s="1"/>
       <c r="R38" s="11"/>
       <c r="S38" s="11"/>
@@ -3365,50 +3500,116 @@
       <c r="U38" s="2"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="22"/>
+      <c r="A39" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>160</v>
+      </c>
       <c r="E39" s="25"/>
       <c r="F39" s="26"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="33"/>
-      <c r="J39" s="31"/>
-      <c r="K39" s="37"/>
-      <c r="L39" s="38"/>
+      <c r="G39" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="H39" s="33">
+        <v>27</v>
+      </c>
+      <c r="I39" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J39" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="K39" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="L39" s="38" t="s">
+        <v>32</v>
+      </c>
       <c r="M39" s="41"/>
-      <c r="N39" s="41"/>
+      <c r="N39" s="41" t="s">
+        <v>81</v>
+      </c>
       <c r="O39" s="40"/>
-      <c r="P39" s="39"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="11"/>
-      <c r="S39" s="11"/>
-      <c r="T39" s="11"/>
-      <c r="U39" s="2"/>
+      <c r="P39" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>6</v>
+      </c>
+      <c r="R39" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="S39" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="T39" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="U39" s="2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="21"/>
+      <c r="A40" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>91</v>
+      </c>
       <c r="D40" s="22"/>
       <c r="E40" s="25"/>
       <c r="F40" s="26"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="33"/>
-      <c r="J40" s="34"/>
-      <c r="K40" s="37"/>
-      <c r="L40" s="38"/>
+      <c r="G40" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="H40" s="33">
+        <v>28</v>
+      </c>
+      <c r="I40" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J40" s="34" t="s">
+        <v>199</v>
+      </c>
+      <c r="K40" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="L40" s="38" t="s">
+        <v>32</v>
+      </c>
       <c r="M40" s="41"/>
-      <c r="N40" s="41"/>
+      <c r="N40" s="41" t="s">
+        <v>63</v>
+      </c>
       <c r="O40" s="40"/>
-      <c r="P40" s="39"/>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="11"/>
-      <c r="S40" s="11"/>
-      <c r="T40" s="11"/>
-      <c r="U40" s="2"/>
+      <c r="P40" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>6</v>
+      </c>
+      <c r="R40" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="S40" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="T40" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="U40" s="2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="19"/>
@@ -3466,7 +3667,7 @@
       <c r="G43" s="32"/>
       <c r="H43" s="33"/>
       <c r="I43" s="33"/>
-      <c r="J43" s="34"/>
+      <c r="J43" s="31"/>
       <c r="K43" s="37"/>
       <c r="L43" s="38"/>
       <c r="M43" s="41"/>
@@ -3502,7 +3703,7 @@
       <c r="T44" s="11"/>
       <c r="U44" s="2"/>
     </row>
-    <row r="45" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="19"/>
       <c r="B45" s="20"/>
       <c r="C45" s="21"/>
@@ -3594,13 +3795,13 @@
       <c r="T48" s="11"/>
       <c r="U48" s="2"/>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="19"/>
       <c r="B49" s="20"/>
       <c r="C49" s="21"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="28"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="26"/>
       <c r="G49" s="32"/>
       <c r="H49" s="33"/>
       <c r="I49" s="33"/>
@@ -3621,9 +3822,9 @@
       <c r="A50" s="19"/>
       <c r="B50" s="20"/>
       <c r="C50" s="21"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="28"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="26"/>
       <c r="G50" s="32"/>
       <c r="H50" s="33"/>
       <c r="I50" s="33"/>
@@ -3644,9 +3845,9 @@
       <c r="A51" s="19"/>
       <c r="B51" s="20"/>
       <c r="C51" s="21"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="28"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="26"/>
       <c r="G51" s="32"/>
       <c r="H51" s="33"/>
       <c r="I51" s="33"/>
@@ -3667,9 +3868,9 @@
       <c r="A52" s="19"/>
       <c r="B52" s="20"/>
       <c r="C52" s="21"/>
-      <c r="D52" s="23"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="28"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="26"/>
       <c r="G52" s="32"/>
       <c r="H52" s="33"/>
       <c r="I52" s="33"/>
@@ -4651,6 +4852,98 @@
       <c r="S94" s="11"/>
       <c r="T94" s="11"/>
       <c r="U94" s="2"/>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A95" s="19"/>
+      <c r="B95" s="20"/>
+      <c r="C95" s="21"/>
+      <c r="D95" s="23"/>
+      <c r="E95" s="27"/>
+      <c r="F95" s="28"/>
+      <c r="G95" s="32"/>
+      <c r="H95" s="33"/>
+      <c r="I95" s="33"/>
+      <c r="J95" s="34"/>
+      <c r="K95" s="37"/>
+      <c r="L95" s="38"/>
+      <c r="M95" s="41"/>
+      <c r="N95" s="41"/>
+      <c r="O95" s="40"/>
+      <c r="P95" s="39"/>
+      <c r="Q95" s="1"/>
+      <c r="R95" s="11"/>
+      <c r="S95" s="11"/>
+      <c r="T95" s="11"/>
+      <c r="U95" s="2"/>
+    </row>
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A96" s="19"/>
+      <c r="B96" s="20"/>
+      <c r="C96" s="21"/>
+      <c r="D96" s="23"/>
+      <c r="E96" s="27"/>
+      <c r="F96" s="28"/>
+      <c r="G96" s="32"/>
+      <c r="H96" s="33"/>
+      <c r="I96" s="33"/>
+      <c r="J96" s="34"/>
+      <c r="K96" s="37"/>
+      <c r="L96" s="38"/>
+      <c r="M96" s="41"/>
+      <c r="N96" s="41"/>
+      <c r="O96" s="40"/>
+      <c r="P96" s="39"/>
+      <c r="Q96" s="1"/>
+      <c r="R96" s="11"/>
+      <c r="S96" s="11"/>
+      <c r="T96" s="11"/>
+      <c r="U96" s="2"/>
+    </row>
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A97" s="19"/>
+      <c r="B97" s="20"/>
+      <c r="C97" s="21"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="27"/>
+      <c r="F97" s="28"/>
+      <c r="G97" s="32"/>
+      <c r="H97" s="33"/>
+      <c r="I97" s="33"/>
+      <c r="J97" s="34"/>
+      <c r="K97" s="37"/>
+      <c r="L97" s="38"/>
+      <c r="M97" s="41"/>
+      <c r="N97" s="41"/>
+      <c r="O97" s="40"/>
+      <c r="P97" s="39"/>
+      <c r="Q97" s="1"/>
+      <c r="R97" s="11"/>
+      <c r="S97" s="11"/>
+      <c r="T97" s="11"/>
+      <c r="U97" s="2"/>
+    </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A98" s="19"/>
+      <c r="B98" s="20"/>
+      <c r="C98" s="21"/>
+      <c r="D98" s="23"/>
+      <c r="E98" s="27"/>
+      <c r="F98" s="28"/>
+      <c r="G98" s="32"/>
+      <c r="H98" s="33"/>
+      <c r="I98" s="33"/>
+      <c r="J98" s="34"/>
+      <c r="K98" s="37"/>
+      <c r="L98" s="38"/>
+      <c r="M98" s="41"/>
+      <c r="N98" s="41"/>
+      <c r="O98" s="40"/>
+      <c r="P98" s="39"/>
+      <c r="Q98" s="1"/>
+      <c r="R98" s="11"/>
+      <c r="S98" s="11"/>
+      <c r="T98" s="11"/>
+      <c r="U98" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="20">

</xml_diff>